<commit_message>
Update news list via RSS
</commit_message>
<xml_diff>
--- a/news_list.xlsx
+++ b/news_list.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,10 +441,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>발행일</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>기사제목</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>링크</t>
         </is>
@@ -453,170 +458,220 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-26 02:05:29</t>
+          <t>2026-01-26 04:12:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>최태원 "지금까지는 서곡일 뿐"…HBM 성공담 담은 '슈퍼모멘텀' 출간</t>
+          <t>2026-01-26 10:00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://magazine.hankyung.com/business/article/202601262433b</t>
+          <t>삼성·LG, 프리미엄 AI 노트북 승자는…신제품 국내 출시</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/003/0013729749?sid=101</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-26 02:05:29</t>
+          <t>2026-01-26 04:12:30</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>고대역폭 메모리(HBM) 성공을 통해 인공지능(AI) 산업의 핵심 플레이어로 거듭난 SK하이닉스의 역사와 최태원 SK그룹 회장의 리더십을 조명한 책이 발간됐다. 26일 업계에 따르면 신간 '슈퍼 모멘텀'(출판사 플랫폼9와3/4)은 어려운 환경을 딛고 SK그룹 편입과 HBM 개발을 통해 AI 시대 주도권을 확보하기까지...</t>
+          <t>2026-01-26 09:48</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://magazine.hankyung.com/business/article/202601262433b</t>
+          <t>구본욱 KB손보 사장 "AI 등 가시적 성과 창출해야"</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/001/0015866302?sid=101</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-26 02:05:29</t>
+          <t>2026-01-26 04:12:30</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>국세청, '착한 소상공인·수출 우수 중기·10년미만 스타드업' 세무조사...</t>
+          <t>2026-01-26 12:01</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.sejungilbo.com/news/articleView.html?idxno=56774</t>
+          <t>갈팡질팡 정부, 결국 ‘대형 원전 건설’로 유턴…AI 전력난 우려에 백...</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/081/0003611658?sid=102</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-26 02:05:29</t>
+          <t>2026-01-26 04:12:30</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>▶ '국세행정 AI 대전환 종합 로드맵' 속도감 있게 수립…국세외수입 징수체계 개편 통합징수 넷째, AI 대전환, 국세외수입 통합징수 등 주요 혁신 과제들을 차질없이 수행해 선제적으로 미래를 준비한다. `27년 본사업 진행을 목표로 '국세행정 AI 대전환 종합 로드맵'을 속도감 있게 수립･추진해나가며 올해는...</t>
+          <t>2026-01-26 06:00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.sejungilbo.com/news/articleView.html?idxno=56774</t>
+          <t>'AI 의료기기' 병원 사용 빨라진다… 최단 80일 만에 진입</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/277/0005711537?sid=101</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-26 02:05:29</t>
+          <t>2026-01-26 04:12:30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>"더 강해지고 세련됐다"… JLR 코리아, 부분변경 모델 '뉴 디펜더' 출시</t>
+          <t>2026-01-26 12:50</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://digitalchosun.dizzo.com/site/data/html_dir/2026/01/26/2026012680091.html</t>
+          <t>삼성 vs. LG, 인공지능(AI) 노트북 신제품 승자는?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>http://woman.chosun.com/news/articleView.html?idxno=124635</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-26 02:05:29</t>
+          <t>2026-01-26 04:12:30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>오디오 선도 기업 서브팩과 협업한 인공지능(AI) 기반 고음질 바이브로-어쿠스틱 기술이 15개 스피커를 갖춘 700W 메리디안 서라운드 사운드 시스템과 함께 작동한다. 웰니스 기능은 다양한 사운드 트랙을 통해 심박수 안정과 인지 향상을 돕는다. 탑승자는 진동 강도를 피비 프로 인포테인먼트 시스템을 통해...</t>
+          <t>2026-01-26 09:36</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://digitalchosun.dizzo.com/site/data/html_dir/2026/01/26/2026012680091.html</t>
+          <t>한국한의약진흥원, 한의약 특화 AI 챗봇 ‘맥챗’ 서비스</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/022/0004100493?sid=102</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-26 02:05:29</t>
+          <t>2026-01-26 04:12:30</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>내부통제 발목 잡힌 윤병운號 NH투자증권, IMA 인가 지연 '발동동'</t>
+          <t>2026-01-26 11:34</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>http://www.shinailbo.co.kr/news/articleView.html?idxno=2182665</t>
+          <t>카카오 그룹, 지역 AI 인재에 답을 묻다</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/018/0006207157?sid=105</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-26 02:05:29</t>
+          <t>2026-01-26 04:12:30</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>이밖에도 인공지능(AI)과 반도체 등 혁신 산업과 중소·중견 기업 투자 및 안정성 등을 고려한 모험자본 투자 포트폴리오도 구축했다. NH투자증권 관계자는 “IMA 사업자가 증가하면서 기업금융 자산에 대한 수요가 빠르게 증가할 것으로 예상된다”면서 “정부의 모험자본 확대 기조에 발맞추고 업계 내...</t>
+          <t>2026-01-26 10:17</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>http://www.shinailbo.co.kr/news/articleView.html?idxno=2182665</t>
+          <t>수자원공사 "오픈AI, AI 물관리 한국과 협력 추진 표명"</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/421/0008734018?sid=102</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-26 02:05:29</t>
+          <t>2026-01-26 04:12:30</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>스쿨플랫, 2026 대한민국 교육박람회 성료…교실 수업에 바로 쓰는 AI 코...</t>
+          <t>2026-01-26 12:53</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.gosiweek.com/article/1065577937648469</t>
+          <t>AI·반도체 전력 수요 급증에...탈원전 폐기</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/016/0002591034?sid=101</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-26 02:05:29</t>
+          <t>2026-01-26 04:12:30</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>스쿨플랫은 교실 수업에 바로 활용할 수 있는 AI 학습 환경으로 교사들의 높은 관심을 받았다. 에듀테크 스타트업 프리윌린(대표 권기성)은 지난 1월 21일부터 23일까지 서울 코엑스에서 열린 ‘2026 대한민국 교육박람회’에 참가해, 초중고 및 대학 교육 현장을 위한 AI 기반 학습·진단 솔루션을 선보이며...</t>
+          <t>2026-01-26 10:52</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.gosiweek.com/article/1065577937648469</t>
+          <t>한국수자원공사, OpenAI와 AI 물관리 모색</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://n.news.naver.com/mnews/article/079/0004108886?sid=102</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto Update: 2026-01-27 05:01:08
</commit_message>
<xml_diff>
--- a/news_list.xlsx
+++ b/news_list.xlsx
@@ -495,22 +495,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>기업</t>
+          <t>기술</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>삼성·LG, 프리미엄 AI 노트북 승자는…신제품 국내 출시</t>
+          <t>마이크로소프트, 차세대 AI 칩 공개···‘탈 엔비디아’ 가속</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013729749?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/032/0003424054?sid=105</t>
         </is>
       </c>
     </row>
@@ -522,12 +522,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>기술</t>
+          <t>정책</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MS도 탈엔비디아 몸부림...성능 30% 높인 AI 추론 칩 출격</t>
+          <t>EU, 머스크 AI 그록 '딥페이크 생성' 조사(종합)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -537,7 +537,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/011/0004583233?sid=104</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015867941?sid=104</t>
         </is>
       </c>
     </row>
@@ -549,22 +549,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>정책</t>
+          <t>기업</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>과기부, 전북서 피지컬 AI 제조혁신 본격화…지역 AX 사업 추진 논의</t>
+          <t>신한금융, 3천500억원 전략 펀드 조성…AI·에너지·인프라 투자</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/022/0004100720?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015868879?sid=105</t>
         </is>
       </c>
     </row>
@@ -576,12 +576,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>정책</t>
+          <t>기업</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>EU, 머스크 AI 그록 '딥페이크 생성' 조사(종합)</t>
+          <t>삼성 AI 랩탑 갤럭시북6 시리즈 출시</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015867941?sid=104</t>
+          <t>https://n.news.naver.com/mnews/article/421/0008736850?sid=105</t>
         </is>
       </c>
     </row>
@@ -603,12 +603,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>기업</t>
+          <t>산업</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>LG CNS, 작년 매출 6조1295억원…AI·클라우드 힘입어 역대 최대 실적</t>
+          <t>의료AI가 사전에 막았다…뷰노 "병원내 심정지 46% ↓"</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -618,7 +618,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013732035?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013731846?sid=102</t>
         </is>
       </c>
     </row>
@@ -630,22 +630,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>산업</t>
+          <t>정책</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>의료AI가 사전에 막았다…뷰노 "병원내 심정지 46% ↓"</t>
+          <t>과기부, 전북서 피지컬 AI 제조혁신 본격화…지역 AX 사업 추진 논의</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013731846?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/022/0004100720?sid=102</t>
         </is>
       </c>
     </row>
@@ -689,7 +689,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>유니온바이오메트릭스, 반려동물 등록 서비스 실증 추진…AI 코 지문 인...</t>
+          <t>[사람과 생각] "기술봉사가 바꾼 인생" 한국기술교육대와의 인연으로 취...</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -699,7 +699,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>http://www.thevaluenews.co.kr/news/view.php?idx=196373</t>
+          <t>https://news.unn.net/news/articleView.html?idxno=589227</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>[독파모] '국가대표 AI' 탈락 논란…기술 경쟁보다 기준 경쟁</t>
+          <t>작년 사이버 침해 신고 2383건···올해 ‘유출 정보 악용’ 위협 전망</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.epnc.co.kr/news/articleView.html?idxno=327760</t>
+          <t>https://n.news.naver.com/mnews/article/032/0003424063?sid=105</t>
         </is>
       </c>
     </row>
@@ -743,7 +743,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>조인철 의원, '네트워크 안정화법' 발의</t>
+          <t>과기정통부·KISA, 2025년 사이버 위협 동향 분석 및 2026년 전망 보고서...</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -753,7 +753,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/277/0005712448?sid=102</t>
+          <t>http://www.metroseoul.co.kr/article/20260127500352</t>
         </is>
       </c>
     </row>
@@ -770,7 +770,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>[S리포트] ①유럽보다 빠른 AI기본법 시대… 득과 실은</t>
+          <t>과기정통부, 피지컬 AI 기반 혁신제품 개발 지원</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -780,7 +780,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/417/0001126626?sid=105</t>
+          <t>https://www.koit.co.kr/news/articleView.html?idxno=205131</t>
         </is>
       </c>
     </row>
@@ -797,7 +797,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>과기정통부, 물리적 인공 지능(피지컬 AI)으로 지역 제조혁신 속도 낸다...</t>
+          <t>중소기업 제조 현장에 인공지능 도입 가속화한다</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -807,7 +807,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://idsn.co.kr/news/view/1065573832923867</t>
+          <t>http://www.ikoreanspirit.com/news/articleView.html?idxno=83678</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto Update: 2026-01-28 04:59:38
</commit_message>
<xml_diff>
--- a/news_list.xlsx
+++ b/news_list.xlsx
@@ -463,223 +463,223 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>기술</t>
+          <t>기업</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[단독] SK하이닉스, 마이크로소프트 차세대 AI칩에 HBM3E 단독 공급</t>
+          <t>오픈AI에 맞불 놓은 구글, 월 1만1000원 저가 AI 요금제 출시</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/009/0005627746?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013734299?sid=105</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>기술</t>
+          <t>기업</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>마이크로소프트, 차세대 AI 칩 공개···‘탈 엔비디아’ 가속</t>
+          <t>구글, 월 1만원선 저가 AI요금제 한·미 등 전세계로 확대</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/032/0003424054?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015870536?sid=104</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>산업</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>'AI 고속도로' 놓는 신한금융, 3500억 전략펀드 조성</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>2026-01-27</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>정책</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>EU, 머스크 AI 그록 '딥페이크 생성' 조사(종합)</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2026-01-27</t>
-        </is>
-      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015867941?sid=104</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013732955?sid=101</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>기업</t>
+          <t>산업</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>신한금융, 3천500억원 전략 펀드 조성…AI·에너지·인프라 투자</t>
+          <t>하나금융, 세종시에 중장년 AI·디지털 일자리센터 열어</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015868879?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015870720?sid=105</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>기업</t>
+          <t>정책</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>삼성 AI 랩탑 갤럭시북6 시리즈 출시</t>
+          <t>[AI픽] 정부, AI 전환에 2.4조 투입…부처 AX 지원 확대</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/421/0008736850?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015870763?sid=105</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>산업</t>
+          <t>정책</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>의료AI가 사전에 막았다…뷰노 "병원내 심정지 46% ↓"</t>
+          <t>[AI픽] AI 기본법 시행, 정부 '스타트업 불안'부터 달랬다</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013731846?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015871238?sid=105</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>기술</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>AI 사용성 강화 갤럭시 북6 울트라·프로 국내 출시 [뉴시스Pic]</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>2026-01-27</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>정책</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>과기부, 전북서 피지컬 AI 제조혁신 본격화…지역 AX 사업 추진 논의</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2026-01-26</t>
-        </is>
-      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/022/0004100720?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013733237?sid=101</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>기술</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>SK하이닉스, MS 차세대 AI 가속기에 HBM '단독 공급'</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>2026-01-27</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>산업</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>"AI가 대신 장 봐드려요" CJ프레시웨이 '프레시엔', AI 주문 기능 도입</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2026-01-27</t>
-        </is>
-      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013731775?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/079/0004109447?sid=101</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -689,24 +689,24 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[사람과 생각] "기술봉사가 바꾼 인생" 한국기술교육대와의 인연으로 취...</t>
+          <t>중앙대, AI 미디어아트로 예당호 관광 콘텐츠 혁신</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://news.unn.net/news/articleView.html?idxno=589227</t>
+          <t>http://www.m-i.kr/news/articleView.html?idxno=1330704</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -716,24 +716,24 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>작년 사이버 침해 신고 2383건···올해 ‘유출 정보 악용’ 위협 전망</t>
+          <t>배경훈 부총리 "AI 경쟁 속도전"···AX예산 2조4000억 투입</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/032/0003424063?sid=105</t>
+          <t>http://www.newsprime.co.kr/news/article.html?no=722075</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -743,24 +743,24 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>과기정통부·KISA, 2025년 사이버 위협 동향 분석 및 2026년 전망 보고서...</t>
+          <t>케이엔에스, 휴머노이드 제어 원천기술 확보 가속</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>http://www.metroseoul.co.kr/article/20260127500352</t>
+          <t>https://www.newspim.com/news/view/20260128000752</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -770,24 +770,24 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>과기정통부, 피지컬 AI 기반 혁신제품 개발 지원</t>
+          <t>전북도, 피지컬AI 확장사업·기업 투자 유치 전략 등 논의…전문가회의...</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.koit.co.kr/news/articleView.html?idxno=205131</t>
+          <t>https://n.news.naver.com/mnews/article/030/0003394111?sid=102</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -797,17 +797,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>중소기업 제조 현장에 인공지능 도입 가속화한다</t>
+          <t>“AI 인류혁명 시대 K-AI 휴머니즘 혁신으로 글로벌 퍼스트무버 발굴 포...</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>http://www.ikoreanspirit.com/news/articleView.html?idxno=83678</t>
+          <t>https://n.news.naver.com/mnews/article/030/0003394106?sid=105</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto Update: 2026-01-29 05:34:30
</commit_message>
<xml_diff>
--- a/news_list.xlsx
+++ b/news_list.xlsx
@@ -463,88 +463,88 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>기업</t>
+          <t>기술</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>오픈AI에 맞불 놓은 구글, 월 1만1000원 저가 AI 요금제 출시</t>
+          <t>"맥락 분석해 오디오 자동 생성"…NC AI, 바르코 사운드 출시</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013734299?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/421/0008741237?sid=105</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>기업</t>
+          <t>기술</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>구글, 월 1만원선 저가 AI요금제 한·미 등 전세계로 확대</t>
+          <t>[AI픽] NC AI, 사운드 생성 인공지능 '바르코 사운드' 출시</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015870536?sid=104</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015872911?sid=105</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>산업</t>
+          <t>정책</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>'AI 고속도로' 놓는 신한금융, 3500억 전략펀드 조성</t>
+          <t>우리은행 "공공기관 AI 전환 지원"…관련 협회와 업무협약</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013732955?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015873297?sid=101</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -554,132 +554,132 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>하나금융, 세종시에 중장년 AI·디지털 일자리센터 열어</t>
+          <t>작년 AI 적용 등 혁신의료기기 45개 지정…전년대비 1.5배</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015870720?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015873367?sid=105</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>기업</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>오픈AI에 맞불 놓은 구글, 월 1만1000원 저가 AI 요금제 출시</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>2026-01-28</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>정책</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>[AI픽] 정부, AI 전환에 2.4조 투입…부처 AX 지원 확대</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2026-01-28</t>
-        </is>
-      </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015870763?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013734299?sid=105</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>정책</t>
+          <t>기업</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[AI픽] AI 기본법 시행, 정부 '스타트업 불안'부터 달랬다</t>
+          <t>충남 천안에 80㎿급 AI 데이터센터 건립…투자협약 체결</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015871238?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015873655?sid=105</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>기술</t>
+          <t>산업</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>AI 사용성 강화 갤럭시 북6 울트라·프로 국내 출시 [뉴시스Pic]</t>
+          <t>"AI 활용 가장 활발했다"…작년 혁신의료기기 45개 지정</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013733237?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013736629?sid=102</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>기술</t>
+          <t>정책</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>SK하이닉스, MS 차세대 AI 가속기에 HBM '단독 공급'</t>
+          <t>우리은행, 공공기관 AI 전환 지원 나선다</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/079/0004109447?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/277/0005713728?sid=101</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -689,24 +689,24 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>중앙대, AI 미디어아트로 예당호 관광 콘텐츠 혁신</t>
+          <t>트릴리온랩스, 국내 첫 확산 기반 트랜스포머 모델 개발</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>http://www.m-i.kr/news/articleView.html?idxno=1330704</t>
+          <t>https://n.news.naver.com/mnews/article/030/0003394619?sid=105</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -716,24 +716,24 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>배경훈 부총리 "AI 경쟁 속도전"···AX예산 2조4000억 투입</t>
+          <t>국내 연구자 호라이즌 유럽 참여 본격화…7개 과제 수주</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>http://www.newsprime.co.kr/news/article.html?no=722075</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015874276?sid=105</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -743,24 +743,24 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>케이엔에스, 휴머노이드 제어 원천기술 확보 가속</t>
+          <t>과기정통부·중기부, AI스타트업 성장전략 설명회 개최</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.newspim.com/news/view/20260128000752</t>
+          <t>https://www.itbiznews.com/news/articleView.html?idxno=202823</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -770,24 +770,24 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>전북도, 피지컬AI 확장사업·기업 투자 유치 전략 등 논의…전문가회의...</t>
+          <t>과기정통부, 양자 분야 첫 마스터플랜 공개…양자인력 1만명·기업 2000개...</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/030/0003394111?sid=102</t>
+          <t>https://www.dailysecu.com/news/articleView.html?idxno=204778</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -797,17 +797,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>“AI 인류혁명 시대 K-AI 휴머니즘 혁신으로 글로벌 퍼스트무버 발굴 포...</t>
+          <t>배경훈 부총리 "AI시대, 양자역할 중요...투자 확대 가속화"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/030/0003394106?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/014/0005470355?sid=105</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto Update: 2026-01-31 05:27:35
</commit_message>
<xml_diff>
--- a/news_list.xlsx
+++ b/news_list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,223 +463,223 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>기술</t>
+          <t>기업</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"맥락 분석해 오디오 자동 생성"…NC AI, 바르코 사운드 출시</t>
+          <t>엔비디아 오픈AI 145조 투자 계획 교착 상태</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/421/0008741237?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013741164?sid=104</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>기술</t>
+          <t>기업</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[AI픽] NC AI, 사운드 생성 인공지능 '바르코 사운드' 출시</t>
+          <t>엔비디아, 오픈AI 145조 투자 보류…"내부 회의론 커져"</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015872911?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/015/0005244994?sid=104</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>정책</t>
+          <t>기술</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>우리은행 "공공기관 AI 전환 지원"…관련 협회와 업무협약</t>
+          <t>정부, 독자AI 모델 기반 '국방 AI' 개발한다</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015873297?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013740053?sid=105</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>산업</t>
+          <t>기술</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>작년 AI 적용 등 혁신의료기기 45개 지정…전년대비 1.5배</t>
+          <t>KT LLM '믿:음' 개발 이끈 최고AI책임자, NC AI로</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015873367?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015876583?sid=105</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>기업</t>
+          <t>산업</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>오픈AI에 맞불 놓은 구글, 월 1만1000원 저가 AI 요금제 출시</t>
+          <t>오세훈 서울시장, 피지컬 AI 거점으로 양재·수서·용산 꼽았다</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013734299?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/277/0005714412?sid=102</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>기업</t>
+          <t>산업</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>충남 천안에 80㎿급 AI 데이터센터 건립…투자협약 체결</t>
+          <t>서울시민 2000명 앞에서 오세훈 시장이 밝힌 피지컬AI 청사진</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015873655?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/277/0005714785?sid=102</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>산업</t>
+          <t>정책</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"AI 활용 가장 활발했다"…작년 혁신의료기기 45개 지정</t>
+          <t>대웅제약, AI 에이전트 활용해 전공의 수련 환경 지원…"행정 감소"</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013736629?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/421/0008744150?sid=103</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>정책</t>
+          <t>정부(과기부)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>우리은행, 공공기관 AI 전환 지원 나선다</t>
+          <t>아크릴, 실시간 로봇 제어 기술로 피지컬 AI 시장 공략</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/277/0005713728?sid=101</t>
+          <t>http://www.technoa.co.kr/news/articleView.html?idxno=100468</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -689,24 +689,24 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>트릴리온랩스, 국내 첫 확산 기반 트랜스포머 모델 개발</t>
+          <t>기후 대응의 해법을 국제 무대에 올린 한밭대</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/030/0003394619?sid=105</t>
+          <t>https://www.ccdailynews.com/news/articleView.html?idxno=2395017</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -716,24 +716,24 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>국내 연구자 호라이즌 유럽 참여 본격화…7개 과제 수주</t>
+          <t>광주시·국토부, 'AI 모빌리티 국가시범도시'본격 추진</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015874276?sid=105</t>
+          <t>http://www.siminsori.com/news/articleView.html?idxno=310069</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -743,24 +743,24 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>과기정통부·중기부, AI스타트업 성장전략 설명회 개최</t>
+          <t>韓 ‘국대 AI’ 제친 4년차 中 ‘스타트업’ 문샷...돌파구는? [김성태의...</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.itbiznews.com/news/articleView.html?idxno=202823</t>
+          <t>https://n.news.naver.com/mnews/article/011/0004585136?sid=105</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -770,44 +770,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>과기정통부, 양자 분야 첫 마스터플랜 공개…양자인력 1만명·기업 2000개...</t>
+          <t>경남, SW미래채움 연차평가 최고등급. . . 7년간 171억 투입</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=204778</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2026-01-29</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>정부(과기부)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>배경훈 부총리 "AI시대, 양자역할 중요...투자 확대 가속화"</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>2026-01-29</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>https://n.news.naver.com/mnews/article/014/0005470355?sid=105</t>
+          <t>https://www.straightnews.co.kr/news/articleView.html?idxno=293779</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto Update: 2026-02-01 06:09:42
</commit_message>
<xml_diff>
--- a/news_list.xlsx
+++ b/news_list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,34 +463,34 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>기업</t>
+          <t>기술</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>엔비디아 오픈AI 145조 투자 계획 교착 상태</t>
+          <t>AI 훈풍 탄 반도체…1월 수출 역대 최고, 흑자 행진</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013741164?sid=104</t>
+          <t>https://n.news.naver.com/mnews/article/005/0001829492?sid=101</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -500,51 +500,51 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>엔비디아, 오픈AI 145조 투자 보류…"내부 회의론 커져"</t>
+          <t>젠슨 황, '오픈AI에 대한 불만설' 부인…"최대 규모 투자할 것"</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/015/0005244994?sid=104</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015877800?sid=104</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>기술</t>
+          <t>기업</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>정부, 독자AI 모델 기반 '국방 AI' 개발한다</t>
+          <t>“오픈AI·엔비디아 145조원 초대형 계약 ‘제동’”…AI동맹 흔들리나</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013740053?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/018/0006210754?sid=101</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -554,7 +554,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>KT LLM '믿:음' 개발 이끈 최고AI책임자, NC AI로</t>
+          <t>정부, 독자AI 모델 기반 '국방 AI' 개발한다</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -564,14 +564,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015876583?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013740053?sid=105</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -581,51 +581,51 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>오세훈 서울시장, 피지컬 AI 거점으로 양재·수서·용산 꼽았다</t>
+          <t>인천항만공사, AI 기반 혁신 우수사례 발굴 주력</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/277/0005714412?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/005/0001829508?sid=102</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>산업</t>
+          <t>정책</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>서울시민 2000명 앞에서 오세훈 시장이 밝힌 피지컬AI 청사진</t>
+          <t>美 'AI규제완화' 슈퍼팩, 중간선거 앞두고 1천800억원 모금</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/277/0005714785?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015878085?sid=104</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -635,51 +635,51 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>대웅제약, AI 에이전트 활용해 전공의 수련 환경 지원…"행정 감소"</t>
+          <t>미 'AI규제완화' 슈퍼팩, 중간선거 앞두고 1천800억 원 모금</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/421/0008744150?sid=103</t>
+          <t>https://n.news.naver.com/mnews/article/055/0001329287?sid=104</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>2026-02-01</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>산업</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[인간과 AI] 의료 현장까지 파고든 AI‥사고시 책임은 누구에게?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>2026-01-31</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>정부(과기부)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>아크릴, 실시간 로봇 제어 기술로 피지컬 AI 시장 공략</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2026-01-31</t>
-        </is>
-      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>http://www.technoa.co.kr/news/articleView.html?idxno=100468</t>
+          <t>https://n.news.naver.com/mnews/article/214/0001477886?sid=102</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -689,24 +689,24 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>기후 대응의 해법을 국제 무대에 올린 한밭대</t>
+          <t>오늘의인사-헌법재판소, 대법원, 국회, 감사원 외</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.ccdailynews.com/news/articleView.html?idxno=2395017</t>
+          <t>https://n.news.naver.com/mnews/article/032/0003425035?sid=102</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -716,24 +716,24 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>광주시·국토부, 'AI 모빌리티 국가시범도시'본격 추진</t>
+          <t>국방 안보, 'K-AI'로 무장…민·관·군 AI 대전환 본격화</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>http://www.siminsori.com/news/articleView.html?idxno=310069</t>
+          <t>https://n.news.naver.com/mnews/article/092/0002408658?sid=105</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -743,24 +743,24 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>韓 ‘국대 AI’ 제친 4년차 中 ‘스타트업’ 문샷...돌파구는? [김성태의...</t>
+          <t>KAIST, 모자처럼 쓰는 탈모 치료기 개발… 光치료 기술, 탈모 치료의 패...</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/011/0004585136?sid=105</t>
+          <t>http://www.biotimes.co.kr/news/articleView.html?idxno=26823</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -770,17 +770,44 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>경남, SW미래채움 연차평가 최고등급. . . 7년간 171억 투입</t>
+          <t>건설연, 국가연구개발 우수성과 100선 선정…“스마트건설기술 상용화”</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.straightnews.co.kr/news/articleView.html?idxno=293779</t>
+          <t>https://n.news.naver.com/mnews/article/666/0000094935?sid=101</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2026-02-01</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>정부(과기부)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>KAIST, 헬맷은 가라...모자처럼 쓰는 탈모 예방 OLED 개발</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2026-02-01</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>http://www.veritas-a.com/news/articleView.html?idxno=596264</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto Update: 2026-02-02 06:43:17
</commit_message>
<xml_diff>
--- a/news_list.xlsx
+++ b/news_list.xlsx
@@ -463,88 +463,88 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>기술</t>
+          <t>산업</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>AI 훈풍 탄 반도체…1월 수출 역대 최고, 흑자 행진</t>
+          <t>대한민국 AI 풀스택, 사우디 시장 진출 본격화</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/005/0001829492?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/031/0001001993?sid=105</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>기업</t>
+          <t>산업</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>젠슨 황, '오픈AI에 대한 불만설' 부인…"최대 규모 투자할 것"</t>
+          <t>주가조작 초동 대응 강화…거래소, AI 시장감시 체계 가동</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015877800?sid=104</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013743257?sid=101</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>기업</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>오픈AI '투자 보류설' 정면 반박한 젠슨 황</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>2026-02-01</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>기업</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>“오픈AI·엔비디아 145조원 초대형 계약 ‘제동’”…AI동맹 흔들리나</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2026-02-01</t>
-        </is>
-      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/018/0006210754?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/015/0005245153?sid=105</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -554,132 +554,132 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>정부, 독자AI 모델 기반 '국방 AI' 개발한다</t>
+          <t>금감원, 가상자산 시세조종 AI로 적발…자동탐지 알고리즘 도입</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013740053?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015879611?sid=101</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>산업</t>
+          <t>정책</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>인천항만공사, AI 기반 혁신 우수사례 발굴 주력</t>
+          <t>산업부, 중견기업 R&amp;D에 655억 투입…"지역 발전·AI 혁신 지원"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/005/0001829508?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015879389?sid=101</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>정책</t>
+          <t>기술</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>美 'AI규제완화' 슈퍼팩, 중간선거 앞두고 1천800억원 모금</t>
+          <t>토스증권, AI 어닝콜 PC버전 출시</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015878085?sid=104</t>
+          <t>https://sports.hankooki.com/news/articleView.html?idxno=6923817</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>기업</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>젠슨 황, 오픈AI '불만설'에 입 열어…"대규모 투자 진행"</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>2026-02-01</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>정책</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>미 'AI규제완화' 슈퍼팩, 중간선거 앞두고 1천800억 원 모금</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2026-02-01</t>
-        </is>
-      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/055/0001329287?sid=104</t>
+          <t>https://n.news.naver.com/mnews/article/015/0005245186?sid=101</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>산업</t>
+          <t>정책</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[인간과 AI] 의료 현장까지 파고든 AI‥사고시 책임은 누구에게?</t>
+          <t>과기부 "한국 AI 풀스택, 사우디 진출 본격화"</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/214/0001477886?sid=102</t>
+          <t>https://n.news.naver.com/mnews/article/215/0001240176?sid=101</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -689,24 +689,24 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>오늘의인사-헌법재판소, 대법원, 국회, 감사원 외</t>
+          <t>가비아, ‘AX 지원 프로모션’…AI 서비스 크레딧 지원</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/032/0003425035?sid=102</t>
+          <t>http://www.datanews.co.kr/news/article.html?no=143146</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -716,24 +716,24 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>국방 안보, 'K-AI'로 무장…민·관·군 AI 대전환 본격화</t>
+          <t>한양대 ERICA AI융합연구소, '연구개발 및 인재 양성 강화 업무협약' 체...</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/092/0002408658?sid=105</t>
+          <t>https://www.kfenews.co.kr/news/articleView.html?idxno=653866</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -743,24 +743,24 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>KAIST, 모자처럼 쓰는 탈모 치료기 개발… 光치료 기술, 탈모 치료의 패...</t>
+          <t>대덕특구 연구소기업 '한다랩', 나스닥 첫 진출 성공</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>http://www.biotimes.co.kr/news/articleView.html?idxno=26823</t>
+          <t>http://www.enewstoday.co.kr/news/articleView.html?idxno=2389438</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -770,24 +770,24 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>건설연, 국가연구개발 우수성과 100선 선정…“스마트건설기술 상용화”</t>
+          <t>한국정보인증, IITP '정보보호 핵심 원천기술 개발사업' 4차년도 과제 성...</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/666/0000094935?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/022/0004102540?sid=101</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -797,17 +797,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>KAIST, 헬맷은 가라...모자처럼 쓰는 탈모 예방 OLED 개발</t>
+          <t>과기부 "한국 AI 풀스택, 사우디 진출 본격화"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>http://www.veritas-a.com/news/articleView.html?idxno=596264</t>
+          <t>https://n.news.naver.com/mnews/article/215/0001240176?sid=101</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto Update: 2026-02-03 06:06:57
</commit_message>
<xml_diff>
--- a/news_list.xlsx
+++ b/news_list.xlsx
@@ -463,61 +463,61 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>산업</t>
+          <t>정책</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>대한민국 AI 풀스택, 사우디 시장 진출 본격화</t>
+          <t>AI기본법 지원데스크, 운영 열흘간 'AI 워터마크' 문의 최다</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/031/0001001993?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013745701?sid=105</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>산업</t>
+          <t>기업</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>주가조작 초동 대응 강화…거래소, AI 시장감시 체계 가동</t>
+          <t>"오픈AI, 엔비디아 칩 성능에 불만"…올트먼-젠슨황 '불협화음'?</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/003/0013743257?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/015/0005246075?sid=105</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -527,24 +527,24 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>오픈AI '투자 보류설' 정면 반박한 젠슨 황</t>
+          <t>스페이스X, xAI 인수…일론 머스크 “우주 기반 AI 시동”</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/015/0005245153?sid=105</t>
+          <t>https://n.news.naver.com/mnews/article/030/0003395691?sid=105</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -554,105 +554,105 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>금감원, 가상자산 시세조종 AI로 적발…자동탐지 알고리즘 도입</t>
+          <t>"AI 메모리도 전월세시대 온다"‥HBM 아버지의 전망</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015879611?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/277/0005716076?sid=101</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>정책</t>
+          <t>기술</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>산업부, 중견기업 R&amp;D에 655억 투입…"지역 발전·AI 혁신 지원"</t>
+          <t>노타, 퓨리오사AI와 AI 모델 최적화 기술 공급 계약 체결</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/001/0015879389?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013746265?sid=105</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>산업</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>'AI로 영구자석 제조 자동화' 한·미 손잡았다</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>2026-02-02</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>기술</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>토스증권, AI 어닝콜 PC버전 출시</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2026-02-02</t>
-        </is>
-      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://sports.hankooki.com/news/articleView.html?idxno=6923817</t>
+          <t>https://n.news.naver.com/mnews/article/015/0005245659?sid=105</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>산업</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>주가조작 초동 대응 강화…거래소, AI 시장감시 체계 가동</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>2026-02-02</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>기업</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>젠슨 황, 오픈AI '불만설'에 입 열어…"대규모 투자 진행"</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2026-02-01</t>
-        </is>
-      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/015/0005245186?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/003/0013743257?sid=101</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -662,24 +662,24 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>과기부 "한국 AI 풀스택, 사우디 진출 본격화"</t>
+          <t>화성시, 공무원 업무 지원 AI 행정비서 'HAI-MATE' 도입</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/215/0001240176?sid=101</t>
+          <t>https://n.news.naver.com/mnews/article/001/0015881761?sid=102</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -689,24 +689,24 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>가비아, ‘AX 지원 프로모션’…AI 서비스 크레딧 지원</t>
+          <t>[의성 소식] 올해 '국가연구개발 우수성과' 100선 선정</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>http://www.datanews.co.kr/news/article.html?no=143146</t>
+          <t>https://n.news.naver.com/mnews/article/417/0001127995?sid=102</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -716,24 +716,24 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>한양대 ERICA AI융합연구소, '연구개발 및 인재 양성 강화 업무협약' 체...</t>
+          <t>뒤늦은 공백 채우기…KAIST·IBS, 수장 선임 절차 '재개'</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.kfenews.co.kr/news/articleView.html?idxno=653866</t>
+          <t>https://n.news.naver.com/mnews/article/008/0005313359?sid=105</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -743,24 +743,24 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>대덕특구 연구소기업 '한다랩', 나스닥 첫 진출 성공</t>
+          <t>의성군 바이오산업단지, 국가연구개발 우수성과 100선 선정</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>http://www.enewstoday.co.kr/news/articleView.html?idxno=2389438</t>
+          <t>https://n.news.naver.com/mnews/article/088/0000995202?sid=102</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -770,24 +770,24 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>한국정보인증, IITP '정보보호 핵심 원천기술 개발사업' 4차년도 과제 성...</t>
+          <t>정부, 2035년 세계 1위 ‘퀀텀칩’ 제조국 노린다</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/022/0004102540?sid=101</t>
+          <t>https://kidd.co.kr/news/244865</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -797,17 +797,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>과기부 "한국 AI 풀스택, 사우디 진출 본격화"</t>
+          <t>블루포인트, 디지털 헬스케어 더마트릭스에 시드 투자 단행</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://n.news.naver.com/mnews/article/215/0001240176?sid=101</t>
+          <t>https://www.news2day.co.kr/article/20260203500192</t>
         </is>
       </c>
     </row>

</xml_diff>